<commit_message>
Added Connections table to lab report
</commit_message>
<xml_diff>
--- a/Connections_Table.xlsx
+++ b/Connections_Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="p1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="60">
   <si>
     <t>Expansion Board J11</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>Motor2(+)</t>
+  </si>
+  <si>
+    <t>POT</t>
+  </si>
+  <si>
+    <t>Expansion Board J11 (34)</t>
+  </si>
+  <si>
+    <t>H-bridge (1) Pot(1)</t>
+  </si>
+  <si>
+    <t>Pot(2)</t>
   </si>
 </sst>
 </file>
@@ -563,26 +575,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +608,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -634,7 +646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -667,7 +679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>6</v>
@@ -707,7 +719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A24" si="0">A4+2</f>
         <v>8</v>
@@ -747,7 +759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -787,7 +799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -827,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -867,7 +879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -907,13 +919,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>13</v>
@@ -947,7 +959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -987,7 +999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1027,7 +1039,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1067,7 +1079,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1107,7 +1119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1147,7 +1159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1187,7 +1199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1227,16 +1239,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
@@ -1267,7 +1279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1289,7 +1301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1312,7 +1324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1333,8 +1345,11 @@
       <c r="G21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1354,8 +1369,17 @@
       <c r="G22" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1376,8 +1400,17 @@
       <c r="G23" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1398,8 +1431,17 @@
       <c r="G24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>A24+2</f>
         <v>48</v>
@@ -1420,8 +1462,17 @@
       <c r="G25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E26">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -1433,7 +1484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E27">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -1445,7 +1496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -1457,7 +1508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1465,7 +1516,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1485,7 +1536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>31</v>
       </c>
@@ -1505,7 +1556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>30</v>
       </c>

</xml_diff>